<commit_message>
File Upload DPLKAKT008-021 until DPLKAKT008-024
</commit_message>
<xml_diff>
--- a/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT008-021 - Akuntansi - Transaksi - Upload Harga Pasar Fixed Income.xlsx
+++ b/Lib_Repo_Excel/FileExcel_DPLK/DPLKAKT008-021 - Akuntansi - Transaksi - Upload Harga Pasar Fixed Income.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1427\Documents\BNI\DPLK\Lib_Repo_Excel\FileExcel_DPLK\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C69F73A7-9641-417B-9611-B5782047143B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC61A794-21F4-40FE-BD55-11E42AE52972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,8 +501,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:W7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,7 +600,7 @@
         <v>25</v>
       </c>
       <c r="G2" s="4">
-        <v>32382</v>
+        <v>32118</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>11</v>

</xml_diff>